<commit_message>
Beginning of Implementation fo Volcano Plot capabilities, and Update of the Install file
</commit_message>
<xml_diff>
--- a/Analysis Temp X vs X/Secondary Analyses/37 C Analysis/Split/CF39 25vs37 vs Lory Data Shrunk2.xlsx
+++ b/Analysis Temp X vs X/Secondary Analyses/37 C Analysis/Split/CF39 25vs37 vs Lory Data Shrunk2.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="290">
   <si>
     <t>locus</t>
   </si>
@@ -913,6 +913,9 @@
   </si>
   <si>
     <t>Fold Change in Lory Analysis 28vs37 (sense)</t>
+  </si>
+  <si>
+    <t>In TnT</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C76" activeCellId="20" sqref="C3 C4 C8 C17 C22 C26 C35 C37 C39 E48 E48 C48 E48 E48 C53 C54 C55 C56 C58 C72 C76"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,7 +3221,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>229</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>233</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>237</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>241</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>245</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>249</v>
       </c>
@@ -3398,7 +3401,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>253</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>257</v>
       </c>
@@ -3455,7 +3458,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>258</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>261</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>268</v>
       </c>
@@ -3544,8 +3547,11 @@
       <c r="I75" s="3">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>271</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>272</v>
       </c>

</xml_diff>